<commit_message>
Fix country name [MK] in Availability tab
</commit_message>
<xml_diff>
--- a/data/Public Availability 2021.xlsx
+++ b/data/Public Availability 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gnat/Workspace/ibp-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399AB939-1692-FA41-AAA3-F23E446BEE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85B054C-E576-8146-9DBF-6B206FC111BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>13</v>
@@ -24324,6 +24324,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6606234b-2704-4bae-93e5-f5741f895a35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="41b5af7a-5d92-4522-a380-16402501482b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C3D97A5466B00649A4CFAAB96F13E5E8" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c515f9dad528904b09be304effe944a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6606234b-2704-4bae-93e5-f5741f895a35" xmlns:ns3="f7643b6f-ebf5-4138-8986-f53ec6ff90c1" xmlns:ns4="41b5af7a-5d92-4522-a380-16402501482b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb4913853e40bb5b15cfd54b985ad66b" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24588,19 +24601,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6606234b-2704-4bae-93e5-f5741f895a35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="41b5af7a-5d92-4522-a380-16402501482b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24611,6 +24611,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42173896-CEC6-46CB-8364-CF7CB87A6B2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="6606234b-2704-4bae-93e5-f5741f895a35"/>
+    <ds:schemaRef ds:uri="41b5af7a-5d92-4522-a380-16402501482b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6213120-3974-4476-9A8A-4F33101DFBB3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24631,18 +24643,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42173896-CEC6-46CB-8364-CF7CB87A6B2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="6606234b-2704-4bae-93e5-f5741f895a35"/>
-    <ds:schemaRef ds:uri="41b5af7a-5d92-4522-a380-16402501482b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B385F753-4590-42EE-AB4A-9EF109D27B02}">
   <ds:schemaRefs>

</xml_diff>